<commit_message>
add code for predicting with RSPB data
</commit_message>
<xml_diff>
--- a/Data/RSPB_data_filtered/RSPB_Data_1999-00_DEC99.xlsx
+++ b/Data/RSPB_data_filtered/RSPB_Data_1999-00_DEC99.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\injg1\Desktop\RSPB Data files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS_CURRENT\SNH_Moray_Firth\SNH_Moray_Firth\Data\RSPB_data_filtered\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5875D5F0-69FA-42E9-986B-AABBC71FEA41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10290" activeTab="2"/>
+    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outer_Dornoch_Firth" sheetId="6" r:id="rId1"/>
     <sheet name="Inverness_Beauly_Firth" sheetId="10" r:id="rId2"/>
     <sheet name="Nairn_Culbin_Bars" sheetId="14" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="79">
   <si>
     <t>Inver</t>
   </si>
@@ -222,9 +233,6 @@
   </si>
   <si>
     <t>NW 1</t>
-  </si>
-  <si>
-    <t>W 1-2</t>
   </si>
   <si>
     <t>Golspie Golf Course</t>
@@ -266,7 +274,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -782,21 +790,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" customHeight="1">
+    <row r="1" spans="1:17" ht="15" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>39</v>
       </c>
@@ -804,55 +811,52 @@
         <v>30</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>32</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="O1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="Q1" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>40</v>
       </c>
@@ -904,11 +908,8 @@
       <c r="Q2" s="16">
         <v>36507</v>
       </c>
-      <c r="R2" s="16">
-        <v>36496</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -960,11 +961,8 @@
       <c r="Q3" s="10">
         <v>0.63541666666666663</v>
       </c>
-      <c r="R3" s="10">
-        <v>0.61111111111111105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>41</v>
       </c>
@@ -1016,11 +1014,8 @@
       <c r="Q4" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="R4" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>42</v>
       </c>
@@ -1072,11 +1067,8 @@
       <c r="Q5" s="18">
         <v>2</v>
       </c>
-      <c r="R5" s="18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>43</v>
       </c>
@@ -1128,11 +1120,8 @@
       <c r="Q6" s="18">
         <v>1</v>
       </c>
-      <c r="R6" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>44</v>
       </c>
@@ -1184,11 +1173,8 @@
       <c r="Q7" s="18">
         <v>1</v>
       </c>
-      <c r="R7" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
@@ -1240,11 +1226,8 @@
       <c r="Q8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="R8" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1272,11 +1255,8 @@
       <c r="O9" s="1"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="10" spans="1:17" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1298,9 +1278,8 @@
       <c r="O10" s="1"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1324,11 +1303,8 @@
       <c r="Q11" s="1">
         <v>1</v>
       </c>
-      <c r="R11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1348,9 +1324,8 @@
       <c r="O12" s="1"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1370,9 +1345,8 @@
       <c r="O13" s="1"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-    </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1392,9 +1366,8 @@
       <c r="O14" s="1"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-    </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1414,9 +1387,8 @@
       <c r="O15" s="1"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-    </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1436,9 +1408,8 @@
       <c r="O16" s="1"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-    </row>
-    <row r="17" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="17" spans="1:17" ht="15" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1458,9 +1429,8 @@
       <c r="O17" s="1"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-    </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="18" spans="1:17" ht="15" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -1490,11 +1460,8 @@
       </c>
       <c r="P18" s="2"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="19" spans="1:17" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -1518,9 +1485,8 @@
       <c r="O19" s="1"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-    </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="20" spans="1:17" ht="15" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1540,9 +1506,8 @@
       <c r="O20" s="1"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="21" spans="1:17" ht="15" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -1562,9 +1527,8 @@
       <c r="O21" s="1"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="22" spans="1:17" ht="15" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -1590,9 +1554,8 @@
         <v>8</v>
       </c>
       <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-    </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="23" spans="1:17" ht="15" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
@@ -1612,9 +1575,8 @@
       <c r="O23" s="1"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-    </row>
-    <row r="24" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="24" spans="1:17" ht="15" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -1634,9 +1596,8 @@
       <c r="O24" s="1"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-    </row>
-    <row r="25" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="25" spans="1:17" ht="15" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
@@ -1656,9 +1617,8 @@
       <c r="O25" s="1"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-    </row>
-    <row r="26" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="26" spans="1:17" ht="15" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1678,9 +1638,8 @@
       <c r="O26" s="1"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-    </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="27" spans="1:17" ht="15" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
@@ -1700,9 +1659,8 @@
       <c r="O27" s="1"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-    </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="28" spans="1:17" ht="15" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
@@ -1722,9 +1680,8 @@
       <c r="O28" s="1"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-    </row>
-    <row r="29" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="29" spans="1:17" ht="15" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
@@ -1748,11 +1705,8 @@
       <c r="O29" s="1"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="30" spans="1:17" ht="15" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -1782,11 +1736,8 @@
       <c r="O30" s="1"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="1"/>
-      <c r="R30" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="31" spans="1:17" ht="15" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -1806,9 +1757,8 @@
       <c r="O31" s="1"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-    </row>
-    <row r="32" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="32" spans="1:17" ht="15" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -1832,9 +1782,8 @@
       <c r="Q32" s="1">
         <v>7</v>
       </c>
-      <c r="R32" s="1"/>
-    </row>
-    <row r="33" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="33" spans="1:17" ht="15" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -1854,9 +1803,8 @@
       <c r="O33" s="1"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-    </row>
-    <row r="34" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="34" spans="1:17" ht="15" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -1876,9 +1824,8 @@
       <c r="O34" s="1"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-    </row>
-    <row r="35" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="35" spans="1:17" ht="15" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
@@ -1898,9 +1845,8 @@
       <c r="O35" s="1"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-    </row>
-    <row r="36" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="36" spans="1:17" ht="15" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -1920,9 +1866,8 @@
       <c r="O36" s="1"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
-    </row>
-    <row r="37" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="37" spans="1:17" ht="15" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1940,9 +1885,8 @@
       <c r="O37" s="1"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-    </row>
-    <row r="38" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="38" spans="1:17" ht="15" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1960,9 +1904,8 @@
       <c r="O38" s="1"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-    </row>
-    <row r="39" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="39" spans="1:17" ht="15" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1980,9 +1923,8 @@
       <c r="O39" s="1"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-    </row>
-    <row r="40" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="40" spans="1:17" ht="15" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2000,9 +1942,8 @@
       <c r="O40" s="1"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-    </row>
-    <row r="41" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="41" spans="1:17" ht="15" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2020,9 +1961,8 @@
       <c r="O41" s="1"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
-    </row>
-    <row r="42" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="42" spans="1:17" ht="15" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
@@ -2040,9 +1980,8 @@
       <c r="O42" s="1"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="1"/>
-      <c r="R42" s="2"/>
-    </row>
-    <row r="43" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="43" spans="1:17" ht="15" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
@@ -2060,9 +1999,8 @@
       <c r="O43" s="1"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="1"/>
-      <c r="R43" s="2"/>
-    </row>
-    <row r="44" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="44" spans="1:17" ht="15" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
@@ -2080,9 +2018,8 @@
       <c r="O44" s="1"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="1"/>
-      <c r="R44" s="2"/>
-    </row>
-    <row r="45" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="45" spans="1:17" ht="15" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="1"/>
@@ -2100,9 +2037,8 @@
       <c r="O45" s="1"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="1"/>
-      <c r="R45" s="2"/>
-    </row>
-    <row r="46" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="46" spans="1:17" ht="15" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="1"/>
@@ -2120,9 +2056,8 @@
       <c r="O46" s="1"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="1"/>
-      <c r="R46" s="2"/>
-    </row>
-    <row r="47" spans="1:18" ht="15" customHeight="1"/>
+    </row>
+    <row r="47" spans="1:17" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.59" right="0.39" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2131,7 +2066,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3501,10 +3436,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>

</xml_diff>